<commit_message>
added the handmeasure data to the chrom class proportion dataset
</commit_message>
<xml_diff>
--- a/data/ChrmClassProportions_melt.xlsx
+++ b/data/ChrmClassProportions_melt.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alpeterson7\Documents\MLH1repo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alpeterson7\Documents\MLH1repo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18225" windowHeight="9720" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18225" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="final_data_sheet" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="melting" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="__Translation_1" localSheetId="1">final_data_sheet!$B$1:$C$1</definedName>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1917" uniqueCount="469">
   <si>
     <t>Original Name</t>
   </si>
@@ -1258,6 +1259,207 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>Original.Name</t>
+  </si>
+  <si>
+    <t>Random.Name</t>
+  </si>
+  <si>
+    <t>18jul19_1mar19_MOLF_m1_sp1_14.1_rev.tif</t>
+  </si>
+  <si>
+    <t>14847-10847-20388.tif</t>
+  </si>
+  <si>
+    <t>18jul19_1mar19_MOLF_m1_sp1_29.1_rev.tif</t>
+  </si>
+  <si>
+    <t>27668-31000-26659.tif</t>
+  </si>
+  <si>
+    <t>18jul19_1mar19_MOLF_m1_sp1_14.2_rev.tif</t>
+  </si>
+  <si>
+    <t>17302-10157-14866.tif</t>
+  </si>
+  <si>
+    <t>18jul19_1mar19_MOLF_m1_sp1_8.3_rev.tif</t>
+  </si>
+  <si>
+    <t>30259-4458-28508.tif</t>
+  </si>
+  <si>
+    <t>18jul19_1mar19_MOLF_m1_sp1_19.1_rev.tif</t>
+  </si>
+  <si>
+    <t>32365-13756-27320.tif</t>
+  </si>
+  <si>
+    <t>18jul19_1mar19_MOLF_m1_sp1_15_rev.tif</t>
+  </si>
+  <si>
+    <t>2967-28380-10176.tif</t>
+  </si>
+  <si>
+    <t>18jul19_1mar19_MOLF_m1_sp1_18_rev.tif</t>
+  </si>
+  <si>
+    <t>23667-10281-6698.tif</t>
+  </si>
+  <si>
+    <t>18jul19_1mar19_MOLF_m1_sp1_11_rev.tif</t>
+  </si>
+  <si>
+    <t>6633-10265-32739.tif</t>
+  </si>
+  <si>
+    <t>18jul19_1mar19_MOLF_m1_sp1_10_rev.tif</t>
+  </si>
+  <si>
+    <t>9033-9283-14583.tif</t>
+  </si>
+  <si>
+    <t>18jul19_1mar19_MOLF_m1_sp1_29.2_rev.tif</t>
+  </si>
+  <si>
+    <t>4463-18484-2583.tif</t>
+  </si>
+  <si>
+    <t>Batch17</t>
+  </si>
+  <si>
+    <t>4nov19_29oct19_MOLF_f1_sp2_9_rev.tif</t>
+  </si>
+  <si>
+    <t>15405-17769-6346.tif</t>
+  </si>
+  <si>
+    <t>4nov19_29oct19_MOLF_f1_sp2_45_rev.tif</t>
+  </si>
+  <si>
+    <t>28976-28312-20715.tif</t>
+  </si>
+  <si>
+    <t>4nov19_29oct19_MOLF_f1_sp2_28_rev.tif</t>
+  </si>
+  <si>
+    <t>28379-17948-3480.tif</t>
+  </si>
+  <si>
+    <t>4nov19_29oct19_MOLF_f1_sp2_46.3_rev.tif</t>
+  </si>
+  <si>
+    <t>25115-32655-28599.tif</t>
+  </si>
+  <si>
+    <t>4nov19_29oct19_MOLF_f1_sp2_16_rev.tif</t>
+  </si>
+  <si>
+    <t>24811-854-605.tif</t>
+  </si>
+  <si>
+    <t>4nov19_29oct19_MOLF_f1_sp2_41_rev.tif</t>
+  </si>
+  <si>
+    <t>5466-31218-1379.tif</t>
+  </si>
+  <si>
+    <t>4nov19_29oct19_MOLF_f1_sp2_6_rev.tif</t>
+  </si>
+  <si>
+    <t>7473-4241-31593.tif</t>
+  </si>
+  <si>
+    <t>4nov19_29oct19_MOLF_f1_sp2_19_rev.tif</t>
+  </si>
+  <si>
+    <t>25026-31368-24706.tif</t>
+  </si>
+  <si>
+    <t>4nov19_29oct19_MOLF_f1_sp2_46.1_rev.tif</t>
+  </si>
+  <si>
+    <t>29698-24444-17917.tif</t>
+  </si>
+  <si>
+    <t>4nov19_29oct19_MOLF_f1_sp2_52_rev.tif</t>
+  </si>
+  <si>
+    <t>2179-20152-2443.tif</t>
+  </si>
+  <si>
+    <t>fix this</t>
+  </si>
+  <si>
+    <t>mean.MLH1.foci</t>
+  </si>
+  <si>
+    <t>mean.MLH1.foci2</t>
+  </si>
+  <si>
+    <t>meanQ</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>G male</t>
+  </si>
+  <si>
+    <t>MOLF male</t>
+  </si>
+  <si>
+    <t>update 12.20.19</t>
+  </si>
+  <si>
+    <t>G female</t>
+  </si>
+  <si>
+    <t>WSB male is missing quant bivs</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>strain</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>AST</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>KAZ</t>
+  </si>
+  <si>
+    <t>LEW</t>
+  </si>
+  <si>
+    <t>MOLF</t>
+  </si>
+  <si>
+    <t>MSM</t>
+  </si>
+  <si>
+    <t>PWD</t>
+  </si>
+  <si>
+    <t>SKIVE</t>
+  </si>
+  <si>
+    <t>TOM</t>
+  </si>
+  <si>
+    <t>WSB</t>
   </si>
 </sst>
 </file>
@@ -1650,24 +1852,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V174"/>
+  <dimension ref="A1:V200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I202" sqref="I202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
     <col min="4" max="4" width="3.5703125" customWidth="1"/>
-    <col min="5" max="6" width="4.28515625" customWidth="1"/>
-    <col min="7" max="7" width="4.28515625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="1.28515625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="5" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="3.85546875" hidden="1" customWidth="1"/>
+    <col min="5" max="7" width="4.28515625" customWidth="1"/>
+    <col min="8" max="8" width="1.28515625" customWidth="1"/>
+    <col min="9" max="9" width="5" customWidth="1"/>
+    <col min="10" max="10" width="3.85546875" customWidth="1"/>
     <col min="11" max="11" width="4.28515625" customWidth="1"/>
     <col min="12" max="13" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="4.28515625" customWidth="1"/>
@@ -9380,6 +9581,826 @@
       <c r="Q174" s="5"/>
       <c r="R174" s="6"/>
     </row>
+    <row r="178" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>376</v>
+      </c>
+      <c r="B178" t="s">
+        <v>402</v>
+      </c>
+      <c r="C178" t="s">
+        <v>403</v>
+      </c>
+      <c r="D178" t="s">
+        <v>2</v>
+      </c>
+      <c r="E178" t="s">
+        <v>119</v>
+      </c>
+      <c r="F178" t="s">
+        <v>4</v>
+      </c>
+      <c r="G178" t="s">
+        <v>5</v>
+      </c>
+      <c r="H178" t="s">
+        <v>6</v>
+      </c>
+      <c r="I178" t="s">
+        <v>7</v>
+      </c>
+      <c r="J178" t="s">
+        <v>8</v>
+      </c>
+      <c r="K178" t="s">
+        <v>9</v>
+      </c>
+      <c r="L178" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M178" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N178" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O178" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P178" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q178" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="R178" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="S178" s="1"/>
+      <c r="T178" s="1"/>
+      <c r="U178" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="179" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="D179" s="1">
+        <v>1</v>
+      </c>
+      <c r="E179" s="1">
+        <v>20</v>
+      </c>
+      <c r="F179" s="1">
+        <v>28</v>
+      </c>
+      <c r="G179" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H179" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I179" s="1">
+        <v>0</v>
+      </c>
+      <c r="J179" s="1">
+        <v>0</v>
+      </c>
+      <c r="L179" s="3">
+        <v>0</v>
+      </c>
+      <c r="M179" s="3">
+        <v>9</v>
+      </c>
+      <c r="N179" s="3">
+        <v>5</v>
+      </c>
+      <c r="O179" s="3">
+        <v>1</v>
+      </c>
+      <c r="P179" s="3"/>
+      <c r="Q179">
+        <f>SUM(L179:P179)</f>
+        <v>15</v>
+      </c>
+      <c r="R179" s="3"/>
+    </row>
+    <row r="180" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>124</v>
+      </c>
+      <c r="B180" t="s">
+        <v>406</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="D180">
+        <v>2</v>
+      </c>
+      <c r="E180">
+        <v>20</v>
+      </c>
+      <c r="F180">
+        <v>25</v>
+      </c>
+      <c r="G180" t="s">
+        <v>10</v>
+      </c>
+      <c r="H180" t="s">
+        <v>11</v>
+      </c>
+      <c r="I180">
+        <v>1</v>
+      </c>
+      <c r="J180">
+        <v>0</v>
+      </c>
+      <c r="L180">
+        <v>1</v>
+      </c>
+      <c r="M180">
+        <v>11</v>
+      </c>
+      <c r="N180">
+        <v>7</v>
+      </c>
+      <c r="Q180">
+        <f>SUM(L180:P180)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="181" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>124</v>
+      </c>
+      <c r="B181" t="s">
+        <v>408</v>
+      </c>
+      <c r="C181" t="s">
+        <v>409</v>
+      </c>
+      <c r="D181">
+        <v>3</v>
+      </c>
+      <c r="E181">
+        <v>20</v>
+      </c>
+      <c r="F181">
+        <v>25</v>
+      </c>
+      <c r="G181" t="s">
+        <v>10</v>
+      </c>
+      <c r="H181" t="s">
+        <v>11</v>
+      </c>
+      <c r="I181">
+        <v>1</v>
+      </c>
+      <c r="J181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>124</v>
+      </c>
+      <c r="B182" t="s">
+        <v>410</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="D182">
+        <v>3</v>
+      </c>
+      <c r="E182">
+        <v>20</v>
+      </c>
+      <c r="F182">
+        <v>25</v>
+      </c>
+      <c r="G182" t="s">
+        <v>10</v>
+      </c>
+      <c r="H182" t="s">
+        <v>11</v>
+      </c>
+      <c r="I182">
+        <v>0</v>
+      </c>
+      <c r="J182">
+        <v>0</v>
+      </c>
+      <c r="L182">
+        <v>1</v>
+      </c>
+      <c r="M182">
+        <v>11</v>
+      </c>
+      <c r="N182">
+        <v>7</v>
+      </c>
+      <c r="Q182">
+        <f t="shared" ref="Q182:Q187" si="148">SUM(L182:P182)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="183" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>124</v>
+      </c>
+      <c r="B183" t="s">
+        <v>412</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="D183">
+        <v>3</v>
+      </c>
+      <c r="E183">
+        <v>20</v>
+      </c>
+      <c r="F183">
+        <v>21</v>
+      </c>
+      <c r="G183" t="s">
+        <v>10</v>
+      </c>
+      <c r="H183" t="s">
+        <v>11</v>
+      </c>
+      <c r="I183">
+        <v>2</v>
+      </c>
+      <c r="J183">
+        <v>0</v>
+      </c>
+      <c r="L183">
+        <v>3</v>
+      </c>
+      <c r="M183">
+        <v>12</v>
+      </c>
+      <c r="N183">
+        <v>4</v>
+      </c>
+      <c r="Q183">
+        <f t="shared" si="148"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="184" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>124</v>
+      </c>
+      <c r="B184" t="s">
+        <v>414</v>
+      </c>
+      <c r="C184" t="s">
+        <v>415</v>
+      </c>
+      <c r="D184">
+        <v>2</v>
+      </c>
+      <c r="E184">
+        <v>20</v>
+      </c>
+      <c r="F184">
+        <v>23</v>
+      </c>
+      <c r="G184" t="s">
+        <v>10</v>
+      </c>
+      <c r="H184" t="s">
+        <v>11</v>
+      </c>
+      <c r="I184">
+        <v>0</v>
+      </c>
+      <c r="J184">
+        <v>0</v>
+      </c>
+      <c r="L184">
+        <v>0</v>
+      </c>
+      <c r="M184">
+        <v>8</v>
+      </c>
+      <c r="N184">
+        <v>11</v>
+      </c>
+      <c r="Q184">
+        <f t="shared" si="148"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="185" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>124</v>
+      </c>
+      <c r="B185" t="s">
+        <v>416</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="D185">
+        <v>3</v>
+      </c>
+      <c r="E185">
+        <v>20</v>
+      </c>
+      <c r="F185">
+        <v>23</v>
+      </c>
+      <c r="G185" t="s">
+        <v>10</v>
+      </c>
+      <c r="H185" t="s">
+        <v>11</v>
+      </c>
+      <c r="I185">
+        <v>0</v>
+      </c>
+      <c r="J185">
+        <v>0</v>
+      </c>
+      <c r="L185">
+        <v>0</v>
+      </c>
+      <c r="M185">
+        <v>15</v>
+      </c>
+      <c r="N185">
+        <v>4</v>
+      </c>
+      <c r="Q185">
+        <f t="shared" si="148"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="186" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>124</v>
+      </c>
+      <c r="B186" t="s">
+        <v>418</v>
+      </c>
+      <c r="C186" t="s">
+        <v>419</v>
+      </c>
+      <c r="D186">
+        <v>2</v>
+      </c>
+      <c r="E186">
+        <v>20</v>
+      </c>
+      <c r="F186">
+        <v>22</v>
+      </c>
+      <c r="G186" t="s">
+        <v>10</v>
+      </c>
+      <c r="H186" t="s">
+        <v>11</v>
+      </c>
+      <c r="I186">
+        <v>0</v>
+      </c>
+      <c r="J186">
+        <v>0</v>
+      </c>
+      <c r="L186">
+        <v>1</v>
+      </c>
+      <c r="M186">
+        <v>11</v>
+      </c>
+      <c r="N186">
+        <v>7</v>
+      </c>
+      <c r="Q186">
+        <f t="shared" si="148"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="187" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>124</v>
+      </c>
+      <c r="B187" t="s">
+        <v>420</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="D187">
+        <v>4</v>
+      </c>
+      <c r="E187">
+        <v>20</v>
+      </c>
+      <c r="F187">
+        <v>24</v>
+      </c>
+      <c r="G187" t="s">
+        <v>10</v>
+      </c>
+      <c r="H187" t="s">
+        <v>11</v>
+      </c>
+      <c r="I187">
+        <v>0</v>
+      </c>
+      <c r="J187">
+        <v>0</v>
+      </c>
+      <c r="L187">
+        <v>1</v>
+      </c>
+      <c r="M187">
+        <v>11</v>
+      </c>
+      <c r="N187">
+        <v>8</v>
+      </c>
+      <c r="O187">
+        <v>0</v>
+      </c>
+      <c r="P187">
+        <v>0</v>
+      </c>
+      <c r="Q187">
+        <f t="shared" si="148"/>
+        <v>20</v>
+      </c>
+      <c r="R187" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="188" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>124</v>
+      </c>
+      <c r="B188" t="s">
+        <v>422</v>
+      </c>
+      <c r="C188" t="s">
+        <v>423</v>
+      </c>
+      <c r="D188">
+        <v>4</v>
+      </c>
+      <c r="E188">
+        <v>20</v>
+      </c>
+      <c r="F188">
+        <v>22</v>
+      </c>
+      <c r="G188" t="s">
+        <v>10</v>
+      </c>
+      <c r="H188" t="s">
+        <v>11</v>
+      </c>
+      <c r="I188">
+        <v>1</v>
+      </c>
+      <c r="J188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>376</v>
+      </c>
+      <c r="B190" t="s">
+        <v>402</v>
+      </c>
+      <c r="C190" t="s">
+        <v>403</v>
+      </c>
+      <c r="D190" t="s">
+        <v>2</v>
+      </c>
+      <c r="E190" t="s">
+        <v>119</v>
+      </c>
+      <c r="F190" t="s">
+        <v>4</v>
+      </c>
+      <c r="G190" t="s">
+        <v>5</v>
+      </c>
+      <c r="H190" t="s">
+        <v>6</v>
+      </c>
+      <c r="I190" t="s">
+        <v>7</v>
+      </c>
+      <c r="J190" t="s">
+        <v>8</v>
+      </c>
+      <c r="K190" t="s">
+        <v>9</v>
+      </c>
+      <c r="L190" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M190" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N190" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O190" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P190" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q190" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="R190" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="S190" s="1"/>
+      <c r="T190" s="1"/>
+      <c r="U190" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="191" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>424</v>
+      </c>
+      <c r="B191" t="s">
+        <v>425</v>
+      </c>
+      <c r="C191" t="s">
+        <v>426</v>
+      </c>
+      <c r="D191">
+        <v>4</v>
+      </c>
+      <c r="E191">
+        <v>20</v>
+      </c>
+      <c r="F191">
+        <v>25</v>
+      </c>
+      <c r="I191">
+        <v>1</v>
+      </c>
+      <c r="J191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>424</v>
+      </c>
+      <c r="B192" t="s">
+        <v>427</v>
+      </c>
+      <c r="C192" t="s">
+        <v>428</v>
+      </c>
+      <c r="D192">
+        <v>2</v>
+      </c>
+      <c r="E192">
+        <v>20</v>
+      </c>
+      <c r="F192">
+        <v>25</v>
+      </c>
+      <c r="I192">
+        <v>0</v>
+      </c>
+      <c r="J192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>424</v>
+      </c>
+      <c r="B193" t="s">
+        <v>429</v>
+      </c>
+      <c r="C193" t="s">
+        <v>430</v>
+      </c>
+      <c r="D193">
+        <v>5</v>
+      </c>
+      <c r="E193">
+        <v>20</v>
+      </c>
+      <c r="F193">
+        <v>25</v>
+      </c>
+      <c r="I193">
+        <v>0</v>
+      </c>
+      <c r="J193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>424</v>
+      </c>
+      <c r="B194" t="s">
+        <v>431</v>
+      </c>
+      <c r="C194" t="s">
+        <v>432</v>
+      </c>
+      <c r="D194">
+        <v>5</v>
+      </c>
+      <c r="E194">
+        <v>20</v>
+      </c>
+      <c r="F194">
+        <v>28</v>
+      </c>
+      <c r="I194">
+        <v>0</v>
+      </c>
+      <c r="J194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>424</v>
+      </c>
+      <c r="B195" t="s">
+        <v>433</v>
+      </c>
+      <c r="C195" t="s">
+        <v>434</v>
+      </c>
+      <c r="D195">
+        <v>4</v>
+      </c>
+      <c r="E195">
+        <v>20</v>
+      </c>
+      <c r="F195">
+        <v>30</v>
+      </c>
+      <c r="I195">
+        <v>0</v>
+      </c>
+      <c r="J195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>424</v>
+      </c>
+      <c r="B196" t="s">
+        <v>435</v>
+      </c>
+      <c r="C196" t="s">
+        <v>436</v>
+      </c>
+      <c r="D196">
+        <v>4</v>
+      </c>
+      <c r="E196">
+        <v>20</v>
+      </c>
+      <c r="F196">
+        <v>20</v>
+      </c>
+      <c r="I196">
+        <v>2</v>
+      </c>
+      <c r="J196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>424</v>
+      </c>
+      <c r="B197" t="s">
+        <v>437</v>
+      </c>
+      <c r="C197" t="s">
+        <v>438</v>
+      </c>
+      <c r="D197">
+        <v>4</v>
+      </c>
+      <c r="E197">
+        <v>20</v>
+      </c>
+      <c r="F197">
+        <v>29</v>
+      </c>
+      <c r="I197">
+        <v>0</v>
+      </c>
+      <c r="J197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>424</v>
+      </c>
+      <c r="B198" t="s">
+        <v>439</v>
+      </c>
+      <c r="C198" t="s">
+        <v>440</v>
+      </c>
+      <c r="D198">
+        <v>3</v>
+      </c>
+      <c r="E198">
+        <v>20</v>
+      </c>
+      <c r="F198">
+        <v>27</v>
+      </c>
+      <c r="I198">
+        <v>0</v>
+      </c>
+      <c r="J198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>424</v>
+      </c>
+      <c r="B199" t="s">
+        <v>441</v>
+      </c>
+      <c r="C199" t="s">
+        <v>442</v>
+      </c>
+      <c r="D199">
+        <v>4</v>
+      </c>
+      <c r="E199">
+        <v>20</v>
+      </c>
+      <c r="F199">
+        <v>26</v>
+      </c>
+      <c r="I199">
+        <v>2</v>
+      </c>
+      <c r="J199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>424</v>
+      </c>
+      <c r="B200" t="s">
+        <v>443</v>
+      </c>
+      <c r="C200" t="s">
+        <v>444</v>
+      </c>
+      <c r="D200">
+        <v>5</v>
+      </c>
+      <c r="E200">
+        <v>20</v>
+      </c>
+      <c r="F200">
+        <v>29</v>
+      </c>
+      <c r="I200">
+        <v>1</v>
+      </c>
+      <c r="J200">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9390,8 +10411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V87"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="S34" sqref="S34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13366,7 +14387,7 @@
         <v>19</v>
       </c>
       <c r="S66">
-        <f t="shared" ref="S66:S97" si="10">R66-F66</f>
+        <f t="shared" ref="S66:S87" si="10">R66-F66</f>
         <v>-1</v>
       </c>
       <c r="T66" t="b">
@@ -14653,13 +15674,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="9" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -14934,7 +15959,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="7" t="s">
         <v>381</v>
       </c>
       <c r="B9" s="6">
@@ -14978,7 +16003,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="7" t="s">
         <v>382</v>
       </c>
       <c r="B10" s="6">
@@ -15285,7 +16310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>389</v>
       </c>
@@ -15329,7 +16354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>390</v>
       </c>
@@ -15371,6 +16396,968 @@
       </c>
       <c r="N18" s="6">
         <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>396</v>
+      </c>
+      <c r="B21" t="s">
+        <v>397</v>
+      </c>
+      <c r="C21" t="s">
+        <v>398</v>
+      </c>
+      <c r="D21" t="s">
+        <v>399</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" t="s">
+        <v>70</v>
+      </c>
+      <c r="J21" t="s">
+        <v>391</v>
+      </c>
+      <c r="K21" t="s">
+        <v>392</v>
+      </c>
+      <c r="L21" t="s">
+        <v>393</v>
+      </c>
+      <c r="M21" t="s">
+        <v>394</v>
+      </c>
+      <c r="N21" t="s">
+        <v>395</v>
+      </c>
+      <c r="O21" t="s">
+        <v>446</v>
+      </c>
+      <c r="P21" t="s">
+        <v>447</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>377</v>
+      </c>
+      <c r="B22">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>120</v>
+      </c>
+      <c r="E22" t="s">
+        <v>449</v>
+      </c>
+      <c r="F22">
+        <v>72</v>
+      </c>
+      <c r="G22">
+        <v>36</v>
+      </c>
+      <c r="H22" t="s">
+        <v>449</v>
+      </c>
+      <c r="I22" t="s">
+        <v>449</v>
+      </c>
+      <c r="J22" t="s">
+        <v>449</v>
+      </c>
+      <c r="K22">
+        <v>0.6</v>
+      </c>
+      <c r="L22">
+        <v>0.3</v>
+      </c>
+      <c r="M22" t="s">
+        <v>449</v>
+      </c>
+      <c r="N22" t="s">
+        <v>449</v>
+      </c>
+      <c r="O22">
+        <v>26.5</v>
+      </c>
+      <c r="P22">
+        <v>28</v>
+      </c>
+      <c r="Q22">
+        <v>2.6666666666666701</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>378</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <v>190</v>
+      </c>
+      <c r="E23" t="s">
+        <v>449</v>
+      </c>
+      <c r="F23">
+        <v>155</v>
+      </c>
+      <c r="G23" t="s">
+        <v>449</v>
+      </c>
+      <c r="H23" t="s">
+        <v>449</v>
+      </c>
+      <c r="I23" t="s">
+        <v>449</v>
+      </c>
+      <c r="J23" t="s">
+        <v>449</v>
+      </c>
+      <c r="K23">
+        <v>0.81578947368421095</v>
+      </c>
+      <c r="L23" t="s">
+        <v>449</v>
+      </c>
+      <c r="M23" t="s">
+        <v>449</v>
+      </c>
+      <c r="N23" t="s">
+        <v>449</v>
+      </c>
+      <c r="O23">
+        <v>21.1</v>
+      </c>
+      <c r="P23">
+        <v>22.5</v>
+      </c>
+      <c r="Q23">
+        <v>2.7</v>
+      </c>
+      <c r="R23" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>453</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>40</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>24</v>
+      </c>
+      <c r="G24">
+        <v>14</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>449</v>
+      </c>
+      <c r="J24">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="K24">
+        <v>0.6</v>
+      </c>
+      <c r="L24">
+        <v>0.35</v>
+      </c>
+      <c r="M24">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="N24" t="s">
+        <v>449</v>
+      </c>
+      <c r="O24">
+        <v>27.5</v>
+      </c>
+      <c r="P24">
+        <v>24.5</v>
+      </c>
+      <c r="Q24">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>450</v>
+      </c>
+      <c r="B25">
+        <v>13</v>
+      </c>
+      <c r="C25">
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <v>247</v>
+      </c>
+      <c r="E25" t="s">
+        <v>449</v>
+      </c>
+      <c r="F25">
+        <v>169</v>
+      </c>
+      <c r="G25">
+        <v>65</v>
+      </c>
+      <c r="H25" t="s">
+        <v>449</v>
+      </c>
+      <c r="I25" t="s">
+        <v>449</v>
+      </c>
+      <c r="J25" t="s">
+        <v>449</v>
+      </c>
+      <c r="K25">
+        <v>0.68421052631578905</v>
+      </c>
+      <c r="L25">
+        <v>0.26315789473684198</v>
+      </c>
+      <c r="M25" t="s">
+        <v>449</v>
+      </c>
+      <c r="N25" t="s">
+        <v>449</v>
+      </c>
+      <c r="O25">
+        <v>23.230769230769202</v>
+      </c>
+      <c r="P25">
+        <v>23.846153846153801</v>
+      </c>
+      <c r="Q25">
+        <v>2.0769230769230802</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>379</v>
+      </c>
+      <c r="B26">
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <v>120</v>
+      </c>
+      <c r="E26">
+        <v>14</v>
+      </c>
+      <c r="F26">
+        <v>76</v>
+      </c>
+      <c r="G26">
+        <v>29</v>
+      </c>
+      <c r="H26" t="s">
+        <v>449</v>
+      </c>
+      <c r="I26" t="s">
+        <v>449</v>
+      </c>
+      <c r="J26">
+        <v>0.116666666666667</v>
+      </c>
+      <c r="K26">
+        <v>0.63333333333333297</v>
+      </c>
+      <c r="L26">
+        <v>0.241666666666667</v>
+      </c>
+      <c r="M26" t="s">
+        <v>449</v>
+      </c>
+      <c r="N26" t="s">
+        <v>449</v>
+      </c>
+      <c r="O26">
+        <v>23</v>
+      </c>
+      <c r="P26">
+        <v>23</v>
+      </c>
+      <c r="Q26">
+        <v>2.3333333333333299</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>380</v>
+      </c>
+      <c r="B27">
+        <v>14</v>
+      </c>
+      <c r="C27">
+        <v>9</v>
+      </c>
+      <c r="D27">
+        <v>266</v>
+      </c>
+      <c r="E27" t="s">
+        <v>449</v>
+      </c>
+      <c r="F27">
+        <v>182</v>
+      </c>
+      <c r="G27">
+        <v>74</v>
+      </c>
+      <c r="H27" t="s">
+        <v>449</v>
+      </c>
+      <c r="I27" t="s">
+        <v>449</v>
+      </c>
+      <c r="J27" t="s">
+        <v>449</v>
+      </c>
+      <c r="K27">
+        <v>0.68421052631578905</v>
+      </c>
+      <c r="L27">
+        <v>0.278195488721804</v>
+      </c>
+      <c r="M27" t="s">
+        <v>449</v>
+      </c>
+      <c r="N27" t="s">
+        <v>449</v>
+      </c>
+      <c r="O27">
+        <v>23.785714285714299</v>
+      </c>
+      <c r="P27">
+        <v>23.5</v>
+      </c>
+      <c r="Q27">
+        <v>2.5714285714285698</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="B28" s="3">
+        <v>10</v>
+      </c>
+      <c r="C28" s="3">
+        <v>7</v>
+      </c>
+      <c r="D28" s="3">
+        <v>142</v>
+      </c>
+      <c r="E28" s="3">
+        <v>5</v>
+      </c>
+      <c r="F28" s="3">
+        <v>97</v>
+      </c>
+      <c r="G28" s="3">
+        <v>35</v>
+      </c>
+      <c r="H28" s="3">
+        <v>4</v>
+      </c>
+      <c r="I28" s="3">
+        <v>1</v>
+      </c>
+      <c r="J28" s="3">
+        <v>3.5211267605633798E-2</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0.68309859154929597</v>
+      </c>
+      <c r="L28" s="3">
+        <v>0.24647887323943701</v>
+      </c>
+      <c r="M28" s="3">
+        <v>2.8169014084507001E-2</v>
+      </c>
+      <c r="N28" s="3">
+        <v>7.0422535211267599E-3</v>
+      </c>
+      <c r="O28" s="3">
+        <v>18.3</v>
+      </c>
+      <c r="P28" s="3">
+        <v>25.8</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B29" s="1">
+        <v>13</v>
+      </c>
+      <c r="C29" s="1">
+        <v>6</v>
+      </c>
+      <c r="D29" s="1">
+        <v>186</v>
+      </c>
+      <c r="E29" s="1">
+        <v>4</v>
+      </c>
+      <c r="F29" s="1">
+        <v>79</v>
+      </c>
+      <c r="G29" s="1">
+        <v>102</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0</v>
+      </c>
+      <c r="J29" s="1">
+        <v>2.1505376344085999E-2</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0.42473118279569899</v>
+      </c>
+      <c r="L29" s="1">
+        <v>0.54838709677419395</v>
+      </c>
+      <c r="M29" s="1">
+        <v>5.3763440860215101E-3</v>
+      </c>
+      <c r="N29" s="1">
+        <v>0</v>
+      </c>
+      <c r="O29" s="1">
+        <v>22</v>
+      </c>
+      <c r="P29" s="1">
+        <v>29.384615384615401</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>2.0769230769230802</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>383</v>
+      </c>
+      <c r="B30">
+        <v>12</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <v>236</v>
+      </c>
+      <c r="E30" t="s">
+        <v>449</v>
+      </c>
+      <c r="F30">
+        <v>137</v>
+      </c>
+      <c r="G30">
+        <v>86</v>
+      </c>
+      <c r="H30" t="s">
+        <v>449</v>
+      </c>
+      <c r="I30" t="s">
+        <v>449</v>
+      </c>
+      <c r="J30" t="s">
+        <v>449</v>
+      </c>
+      <c r="K30">
+        <v>0.58050847457627097</v>
+      </c>
+      <c r="L30">
+        <v>0.36440677966101698</v>
+      </c>
+      <c r="M30" t="s">
+        <v>449</v>
+      </c>
+      <c r="N30" t="s">
+        <v>449</v>
+      </c>
+      <c r="O30">
+        <v>27.5</v>
+      </c>
+      <c r="P30">
+        <v>28.5833333333333</v>
+      </c>
+      <c r="Q30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>384</v>
+      </c>
+      <c r="B31">
+        <v>18</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>333</v>
+      </c>
+      <c r="E31" t="s">
+        <v>449</v>
+      </c>
+      <c r="F31">
+        <v>140</v>
+      </c>
+      <c r="G31">
+        <v>179</v>
+      </c>
+      <c r="H31" t="s">
+        <v>449</v>
+      </c>
+      <c r="I31" t="s">
+        <v>449</v>
+      </c>
+      <c r="J31" t="s">
+        <v>449</v>
+      </c>
+      <c r="K31">
+        <v>0.42042042042041999</v>
+      </c>
+      <c r="L31">
+        <v>0.53753753753753797</v>
+      </c>
+      <c r="M31" t="s">
+        <v>449</v>
+      </c>
+      <c r="N31" t="s">
+        <v>449</v>
+      </c>
+      <c r="O31">
+        <v>29.3333333333333</v>
+      </c>
+      <c r="P31">
+        <v>30.3888888888889</v>
+      </c>
+      <c r="Q31">
+        <v>1.94444444444444</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>451</v>
+      </c>
+      <c r="B32">
+        <v>6</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>114</v>
+      </c>
+      <c r="E32">
+        <v>6</v>
+      </c>
+      <c r="F32">
+        <v>68</v>
+      </c>
+      <c r="G32">
+        <v>40</v>
+      </c>
+      <c r="H32" t="s">
+        <v>449</v>
+      </c>
+      <c r="I32" t="s">
+        <v>449</v>
+      </c>
+      <c r="J32">
+        <v>5.2631578947368397E-2</v>
+      </c>
+      <c r="K32">
+        <v>0.59649122807017496</v>
+      </c>
+      <c r="L32">
+        <v>0.35087719298245601</v>
+      </c>
+      <c r="M32" t="s">
+        <v>449</v>
+      </c>
+      <c r="N32" t="s">
+        <v>449</v>
+      </c>
+      <c r="O32">
+        <v>24.6666666666667</v>
+      </c>
+      <c r="P32">
+        <v>23.1666666666667</v>
+      </c>
+      <c r="Q32">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B33" s="1">
+        <v>10</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>179</v>
+      </c>
+      <c r="E33" s="1">
+        <v>3</v>
+      </c>
+      <c r="F33" s="1">
+        <v>107</v>
+      </c>
+      <c r="G33" s="1">
+        <v>67</v>
+      </c>
+      <c r="H33" s="1">
+        <v>2</v>
+      </c>
+      <c r="I33" s="1">
+        <v>0</v>
+      </c>
+      <c r="J33" s="1">
+        <v>1.67597765363128E-2</v>
+      </c>
+      <c r="K33" s="1">
+        <v>0.59776536312849204</v>
+      </c>
+      <c r="L33" s="1">
+        <v>0.37430167597765401</v>
+      </c>
+      <c r="M33" s="1">
+        <v>1.11731843575419E-2</v>
+      </c>
+      <c r="N33" s="1">
+        <v>0</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="P33" s="1">
+        <v>28.3</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>386</v>
+      </c>
+      <c r="B34">
+        <v>7</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>132</v>
+      </c>
+      <c r="E34" t="s">
+        <v>449</v>
+      </c>
+      <c r="F34">
+        <v>72</v>
+      </c>
+      <c r="G34">
+        <v>58</v>
+      </c>
+      <c r="H34" t="s">
+        <v>449</v>
+      </c>
+      <c r="I34" t="s">
+        <v>449</v>
+      </c>
+      <c r="J34" t="s">
+        <v>449</v>
+      </c>
+      <c r="K34">
+        <v>0.54545454545454497</v>
+      </c>
+      <c r="L34">
+        <v>0.439393939393939</v>
+      </c>
+      <c r="M34" t="s">
+        <v>449</v>
+      </c>
+      <c r="N34" t="s">
+        <v>449</v>
+      </c>
+      <c r="O34">
+        <v>27.285714285714299</v>
+      </c>
+      <c r="P34">
+        <v>26.8571428571429</v>
+      </c>
+      <c r="Q34">
+        <v>2.8571428571428599</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>387</v>
+      </c>
+      <c r="B35">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>160</v>
+      </c>
+      <c r="E35" t="s">
+        <v>449</v>
+      </c>
+      <c r="F35">
+        <v>108</v>
+      </c>
+      <c r="G35">
+        <v>43</v>
+      </c>
+      <c r="H35" t="s">
+        <v>449</v>
+      </c>
+      <c r="I35" t="s">
+        <v>449</v>
+      </c>
+      <c r="J35" t="s">
+        <v>449</v>
+      </c>
+      <c r="K35">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="L35">
+        <v>0.26874999999999999</v>
+      </c>
+      <c r="M35" t="s">
+        <v>449</v>
+      </c>
+      <c r="N35" t="s">
+        <v>449</v>
+      </c>
+      <c r="O35">
+        <v>25.375</v>
+      </c>
+      <c r="P35">
+        <v>24.5</v>
+      </c>
+      <c r="Q35">
+        <v>2.625</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>388</v>
+      </c>
+      <c r="B36">
+        <v>6</v>
+      </c>
+      <c r="C36">
+        <v>5</v>
+      </c>
+      <c r="D36">
+        <v>113</v>
+      </c>
+      <c r="E36" t="s">
+        <v>449</v>
+      </c>
+      <c r="F36">
+        <v>89</v>
+      </c>
+      <c r="G36">
+        <v>19</v>
+      </c>
+      <c r="H36" t="s">
+        <v>449</v>
+      </c>
+      <c r="I36" t="s">
+        <v>449</v>
+      </c>
+      <c r="J36" t="s">
+        <v>449</v>
+      </c>
+      <c r="K36">
+        <v>0.787610619469027</v>
+      </c>
+      <c r="L36">
+        <v>0.16814159292035399</v>
+      </c>
+      <c r="M36" t="s">
+        <v>449</v>
+      </c>
+      <c r="N36" t="s">
+        <v>449</v>
+      </c>
+      <c r="O36">
+        <v>21.6666666666667</v>
+      </c>
+      <c r="P36">
+        <v>21.5</v>
+      </c>
+      <c r="Q36">
+        <v>2.3333333333333299</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>389</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>57</v>
+      </c>
+      <c r="E37" t="s">
+        <v>449</v>
+      </c>
+      <c r="F37">
+        <v>39</v>
+      </c>
+      <c r="G37">
+        <v>16</v>
+      </c>
+      <c r="H37" t="s">
+        <v>449</v>
+      </c>
+      <c r="I37" t="s">
+        <v>449</v>
+      </c>
+      <c r="J37" t="s">
+        <v>449</v>
+      </c>
+      <c r="K37">
+        <v>0.68421052631578905</v>
+      </c>
+      <c r="L37">
+        <v>0.28070175438596501</v>
+      </c>
+      <c r="M37" t="s">
+        <v>449</v>
+      </c>
+      <c r="N37" t="s">
+        <v>449</v>
+      </c>
+      <c r="O37">
+        <v>23.6666666666667</v>
+      </c>
+      <c r="P37">
+        <v>24</v>
+      </c>
+      <c r="Q37">
+        <v>2.3333333333333299</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>390</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>38</v>
+      </c>
+      <c r="E38" t="s">
+        <v>449</v>
+      </c>
+      <c r="F38">
+        <v>24</v>
+      </c>
+      <c r="G38">
+        <v>13</v>
+      </c>
+      <c r="H38" t="s">
+        <v>449</v>
+      </c>
+      <c r="I38" t="s">
+        <v>449</v>
+      </c>
+      <c r="J38" t="s">
+        <v>449</v>
+      </c>
+      <c r="K38">
+        <v>0.63157894736842102</v>
+      </c>
+      <c r="L38">
+        <v>0.34210526315789502</v>
+      </c>
+      <c r="M38" t="s">
+        <v>449</v>
+      </c>
+      <c r="N38" t="s">
+        <v>449</v>
+      </c>
+      <c r="O38">
+        <v>25</v>
+      </c>
+      <c r="P38">
+        <v>27</v>
+      </c>
+      <c r="Q38">
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>
@@ -15381,15 +17368,1519 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:V86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D1" t="s">
+        <v>455</v>
+      </c>
+      <c r="E1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C2" t="s">
+        <v>449</v>
+      </c>
+      <c r="D2" t="s">
+        <v>457</v>
+      </c>
+      <c r="E2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>389</v>
+      </c>
+      <c r="B3" t="s">
+        <v>392</v>
+      </c>
+      <c r="C3">
+        <v>0.68421052631578905</v>
+      </c>
+      <c r="D3" t="s">
+        <v>457</v>
+      </c>
+      <c r="E3" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>389</v>
+      </c>
+      <c r="B4" t="s">
+        <v>393</v>
+      </c>
+      <c r="C4">
+        <v>0.28070175438596501</v>
+      </c>
+      <c r="D4" t="s">
+        <v>457</v>
+      </c>
+      <c r="E4" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>389</v>
+      </c>
+      <c r="B5" t="s">
+        <v>394</v>
+      </c>
+      <c r="C5" t="s">
+        <v>449</v>
+      </c>
+      <c r="D5" t="s">
+        <v>457</v>
+      </c>
+      <c r="E5" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>389</v>
+      </c>
+      <c r="B6" t="s">
+        <v>395</v>
+      </c>
+      <c r="C6" t="s">
+        <v>449</v>
+      </c>
+      <c r="D6" t="s">
+        <v>457</v>
+      </c>
+      <c r="E6" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>453</v>
+      </c>
+      <c r="B7" t="s">
+        <v>391</v>
+      </c>
+      <c r="C7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>458</v>
+      </c>
+      <c r="E7" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>453</v>
+      </c>
+      <c r="B8" t="s">
+        <v>392</v>
+      </c>
+      <c r="C8">
+        <v>0.6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>458</v>
+      </c>
+      <c r="E8" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>453</v>
+      </c>
+      <c r="B9" t="s">
+        <v>393</v>
+      </c>
+      <c r="C9">
+        <v>0.35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>458</v>
+      </c>
+      <c r="E9" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>453</v>
+      </c>
+      <c r="B10" t="s">
+        <v>394</v>
+      </c>
+      <c r="C10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>458</v>
+      </c>
+      <c r="E10" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>453</v>
+      </c>
+      <c r="B11" t="s">
+        <v>395</v>
+      </c>
+      <c r="C11" t="s">
+        <v>449</v>
+      </c>
+      <c r="D11" t="s">
+        <v>458</v>
+      </c>
+      <c r="E11" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>450</v>
+      </c>
+      <c r="B12" t="s">
+        <v>391</v>
+      </c>
+      <c r="C12" t="s">
+        <v>449</v>
+      </c>
+      <c r="D12" t="s">
+        <v>457</v>
+      </c>
+      <c r="E12" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>450</v>
+      </c>
+      <c r="B13" t="s">
+        <v>392</v>
+      </c>
+      <c r="C13">
+        <v>0.68421052631578905</v>
+      </c>
+      <c r="D13" t="s">
+        <v>457</v>
+      </c>
+      <c r="E13" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>450</v>
+      </c>
+      <c r="B14" t="s">
+        <v>393</v>
+      </c>
+      <c r="C14">
+        <v>0.26315789473684198</v>
+      </c>
+      <c r="D14" t="s">
+        <v>457</v>
+      </c>
+      <c r="E14" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>450</v>
+      </c>
+      <c r="B15" t="s">
+        <v>394</v>
+      </c>
+      <c r="C15" t="s">
+        <v>449</v>
+      </c>
+      <c r="D15" t="s">
+        <v>457</v>
+      </c>
+      <c r="E15" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>450</v>
+      </c>
+      <c r="B16" t="s">
+        <v>395</v>
+      </c>
+      <c r="C16" t="s">
+        <v>449</v>
+      </c>
+      <c r="D16" t="s">
+        <v>457</v>
+      </c>
+      <c r="E16" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>387</v>
+      </c>
+      <c r="B17" t="s">
+        <v>391</v>
+      </c>
+      <c r="C17" t="s">
+        <v>449</v>
+      </c>
+      <c r="D17" t="s">
+        <v>458</v>
+      </c>
+      <c r="E17" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>387</v>
+      </c>
+      <c r="B18" t="s">
+        <v>392</v>
+      </c>
+      <c r="C18">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="D18" t="s">
+        <v>458</v>
+      </c>
+      <c r="E18" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>387</v>
+      </c>
+      <c r="B19" t="s">
+        <v>393</v>
+      </c>
+      <c r="C19">
+        <v>0.26874999999999999</v>
+      </c>
+      <c r="D19" t="s">
+        <v>458</v>
+      </c>
+      <c r="E19" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>387</v>
+      </c>
+      <c r="B20" t="s">
+        <v>394</v>
+      </c>
+      <c r="C20" t="s">
+        <v>449</v>
+      </c>
+      <c r="D20" t="s">
+        <v>458</v>
+      </c>
+      <c r="E20" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>387</v>
+      </c>
+      <c r="B21" t="s">
+        <v>395</v>
+      </c>
+      <c r="C21" t="s">
+        <v>449</v>
+      </c>
+      <c r="D21" t="s">
+        <v>458</v>
+      </c>
+      <c r="E21" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>388</v>
+      </c>
+      <c r="B22" t="s">
+        <v>391</v>
+      </c>
+      <c r="C22" t="s">
+        <v>449</v>
+      </c>
+      <c r="D22" t="s">
+        <v>457</v>
+      </c>
+      <c r="E22" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>388</v>
+      </c>
+      <c r="B23" t="s">
+        <v>392</v>
+      </c>
+      <c r="C23">
+        <v>0.787610619469027</v>
+      </c>
+      <c r="D23" t="s">
+        <v>457</v>
+      </c>
+      <c r="E23" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>388</v>
+      </c>
+      <c r="B24" t="s">
+        <v>393</v>
+      </c>
+      <c r="C24">
+        <v>0.16814159292035399</v>
+      </c>
+      <c r="D24" t="s">
+        <v>457</v>
+      </c>
+      <c r="E24" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>388</v>
+      </c>
+      <c r="B25" t="s">
+        <v>394</v>
+      </c>
+      <c r="C25" t="s">
+        <v>449</v>
+      </c>
+      <c r="D25" t="s">
+        <v>457</v>
+      </c>
+      <c r="E25" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B26" t="s">
+        <v>395</v>
+      </c>
+      <c r="C26" t="s">
+        <v>449</v>
+      </c>
+      <c r="D26" t="s">
+        <v>457</v>
+      </c>
+      <c r="E26" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>379</v>
+      </c>
+      <c r="B27" t="s">
+        <v>391</v>
+      </c>
+      <c r="C27">
+        <v>0.116666666666667</v>
+      </c>
+      <c r="D27" t="s">
+        <v>458</v>
+      </c>
+      <c r="E27" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>379</v>
+      </c>
+      <c r="B28" t="s">
+        <v>392</v>
+      </c>
+      <c r="C28">
+        <v>0.63333333333333297</v>
+      </c>
+      <c r="D28" t="s">
+        <v>458</v>
+      </c>
+      <c r="E28" t="s">
+        <v>462</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>379</v>
+      </c>
+      <c r="B29" t="s">
+        <v>393</v>
+      </c>
+      <c r="C29">
+        <v>0.241666666666667</v>
+      </c>
+      <c r="D29" t="s">
+        <v>458</v>
+      </c>
+      <c r="E29" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>379</v>
+      </c>
+      <c r="B30" t="s">
+        <v>394</v>
+      </c>
+      <c r="C30" t="s">
+        <v>449</v>
+      </c>
+      <c r="D30" t="s">
+        <v>458</v>
+      </c>
+      <c r="E30" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>379</v>
+      </c>
+      <c r="B31" t="s">
+        <v>395</v>
+      </c>
+      <c r="C31" t="s">
+        <v>449</v>
+      </c>
+      <c r="D31" t="s">
+        <v>458</v>
+      </c>
+      <c r="E31" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>380</v>
+      </c>
+      <c r="B32" t="s">
+        <v>391</v>
+      </c>
+      <c r="C32" t="s">
+        <v>449</v>
+      </c>
+      <c r="D32" t="s">
+        <v>457</v>
+      </c>
+      <c r="E32" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>380</v>
+      </c>
+      <c r="B33" t="s">
+        <v>392</v>
+      </c>
+      <c r="C33">
+        <v>0.68421052631578905</v>
+      </c>
+      <c r="D33" t="s">
+        <v>457</v>
+      </c>
+      <c r="E33" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>380</v>
+      </c>
+      <c r="B34" t="s">
+        <v>393</v>
+      </c>
+      <c r="C34">
+        <v>0.278195488721804</v>
+      </c>
+      <c r="D34" t="s">
+        <v>457</v>
+      </c>
+      <c r="E34" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>380</v>
+      </c>
+      <c r="B35" t="s">
+        <v>394</v>
+      </c>
+      <c r="C35" t="s">
+        <v>449</v>
+      </c>
+      <c r="D35" t="s">
+        <v>457</v>
+      </c>
+      <c r="E35" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>380</v>
+      </c>
+      <c r="B36" t="s">
+        <v>395</v>
+      </c>
+      <c r="C36" t="s">
+        <v>449</v>
+      </c>
+      <c r="D36" t="s">
+        <v>457</v>
+      </c>
+      <c r="E36" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>451</v>
+      </c>
+      <c r="B37" t="s">
+        <v>391</v>
+      </c>
+      <c r="C37">
+        <v>5.2631578947368397E-2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>457</v>
+      </c>
+      <c r="E37" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>451</v>
+      </c>
+      <c r="B38" t="s">
+        <v>392</v>
+      </c>
+      <c r="C38">
+        <v>0.59649122807017496</v>
+      </c>
+      <c r="D38" t="s">
+        <v>457</v>
+      </c>
+      <c r="E38" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>451</v>
+      </c>
+      <c r="B39" t="s">
+        <v>393</v>
+      </c>
+      <c r="C39">
+        <v>0.35087719298245601</v>
+      </c>
+      <c r="D39" t="s">
+        <v>457</v>
+      </c>
+      <c r="E39" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>451</v>
+      </c>
+      <c r="B40" t="s">
+        <v>394</v>
+      </c>
+      <c r="C40" t="s">
+        <v>449</v>
+      </c>
+      <c r="D40" t="s">
+        <v>457</v>
+      </c>
+      <c r="E40" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>451</v>
+      </c>
+      <c r="B41" t="s">
+        <v>395</v>
+      </c>
+      <c r="C41" t="s">
+        <v>449</v>
+      </c>
+      <c r="D41" t="s">
+        <v>457</v>
+      </c>
+      <c r="E41" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>383</v>
+      </c>
+      <c r="B42" t="s">
+        <v>391</v>
+      </c>
+      <c r="C42" t="s">
+        <v>449</v>
+      </c>
+      <c r="D42" t="s">
+        <v>458</v>
+      </c>
+      <c r="E42" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>383</v>
+      </c>
+      <c r="B43" t="s">
+        <v>392</v>
+      </c>
+      <c r="C43">
+        <v>0.58050847457627097</v>
+      </c>
+      <c r="D43" t="s">
+        <v>458</v>
+      </c>
+      <c r="E43" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>383</v>
+      </c>
+      <c r="B44" t="s">
+        <v>393</v>
+      </c>
+      <c r="C44">
+        <v>0.36440677966101698</v>
+      </c>
+      <c r="D44" t="s">
+        <v>458</v>
+      </c>
+      <c r="E44" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>383</v>
+      </c>
+      <c r="B45" t="s">
+        <v>394</v>
+      </c>
+      <c r="C45" t="s">
+        <v>449</v>
+      </c>
+      <c r="D45" t="s">
+        <v>458</v>
+      </c>
+      <c r="E45" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>383</v>
+      </c>
+      <c r="B46" t="s">
+        <v>395</v>
+      </c>
+      <c r="C46" t="s">
+        <v>449</v>
+      </c>
+      <c r="D46" t="s">
+        <v>458</v>
+      </c>
+      <c r="E46" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>384</v>
+      </c>
+      <c r="B47" t="s">
+        <v>391</v>
+      </c>
+      <c r="C47" t="s">
+        <v>449</v>
+      </c>
+      <c r="D47" t="s">
+        <v>457</v>
+      </c>
+      <c r="E47" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>384</v>
+      </c>
+      <c r="B48" t="s">
+        <v>392</v>
+      </c>
+      <c r="C48">
+        <v>0.42042042042041999</v>
+      </c>
+      <c r="D48" t="s">
+        <v>457</v>
+      </c>
+      <c r="E48" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>384</v>
+      </c>
+      <c r="B49" t="s">
+        <v>393</v>
+      </c>
+      <c r="C49">
+        <v>0.53753753753753797</v>
+      </c>
+      <c r="D49" t="s">
+        <v>457</v>
+      </c>
+      <c r="E49" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>384</v>
+      </c>
+      <c r="B50" t="s">
+        <v>394</v>
+      </c>
+      <c r="C50" t="s">
+        <v>449</v>
+      </c>
+      <c r="D50" t="s">
+        <v>457</v>
+      </c>
+      <c r="E50" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>384</v>
+      </c>
+      <c r="B51" t="s">
+        <v>395</v>
+      </c>
+      <c r="C51" t="s">
+        <v>449</v>
+      </c>
+      <c r="D51" t="s">
+        <v>457</v>
+      </c>
+      <c r="E51" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>381</v>
+      </c>
+      <c r="B52" t="s">
+        <v>391</v>
+      </c>
+      <c r="C52" t="s">
+        <v>449</v>
+      </c>
+      <c r="D52" t="s">
+        <v>458</v>
+      </c>
+      <c r="E52" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>381</v>
+      </c>
+      <c r="B53" t="s">
+        <v>392</v>
+      </c>
+      <c r="C53" t="s">
+        <v>449</v>
+      </c>
+      <c r="D53" t="s">
+        <v>458</v>
+      </c>
+      <c r="E53" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>381</v>
+      </c>
+      <c r="B54" t="s">
+        <v>393</v>
+      </c>
+      <c r="C54" t="s">
+        <v>449</v>
+      </c>
+      <c r="D54" t="s">
+        <v>458</v>
+      </c>
+      <c r="E54" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>381</v>
+      </c>
+      <c r="B55" t="s">
+        <v>394</v>
+      </c>
+      <c r="C55" t="s">
+        <v>449</v>
+      </c>
+      <c r="D55" t="s">
+        <v>458</v>
+      </c>
+      <c r="E55" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>381</v>
+      </c>
+      <c r="B56" t="s">
+        <v>395</v>
+      </c>
+      <c r="C56" t="s">
+        <v>449</v>
+      </c>
+      <c r="D56" t="s">
+        <v>458</v>
+      </c>
+      <c r="E56" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>382</v>
+      </c>
+      <c r="B57" t="s">
+        <v>391</v>
+      </c>
+      <c r="C57" t="s">
+        <v>449</v>
+      </c>
+      <c r="D57" t="s">
+        <v>457</v>
+      </c>
+      <c r="E57" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>382</v>
+      </c>
+      <c r="B58" t="s">
+        <v>392</v>
+      </c>
+      <c r="C58" t="s">
+        <v>449</v>
+      </c>
+      <c r="D58" t="s">
+        <v>457</v>
+      </c>
+      <c r="E58" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>382</v>
+      </c>
+      <c r="B59" t="s">
+        <v>393</v>
+      </c>
+      <c r="C59" t="s">
+        <v>449</v>
+      </c>
+      <c r="D59" t="s">
+        <v>457</v>
+      </c>
+      <c r="E59" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>382</v>
+      </c>
+      <c r="B60" t="s">
+        <v>394</v>
+      </c>
+      <c r="C60" t="s">
+        <v>449</v>
+      </c>
+      <c r="D60" t="s">
+        <v>457</v>
+      </c>
+      <c r="E60" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>382</v>
+      </c>
+      <c r="B61" t="s">
+        <v>395</v>
+      </c>
+      <c r="C61" t="s">
+        <v>449</v>
+      </c>
+      <c r="D61" t="s">
+        <v>457</v>
+      </c>
+      <c r="E61" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>385</v>
+      </c>
+      <c r="B62" t="s">
+        <v>391</v>
+      </c>
+      <c r="C62" t="s">
+        <v>449</v>
+      </c>
+      <c r="D62" t="s">
+        <v>458</v>
+      </c>
+      <c r="E62" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>385</v>
+      </c>
+      <c r="B63" t="s">
+        <v>392</v>
+      </c>
+      <c r="C63" t="s">
+        <v>449</v>
+      </c>
+      <c r="D63" t="s">
+        <v>458</v>
+      </c>
+      <c r="E63" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>385</v>
+      </c>
+      <c r="B64" t="s">
+        <v>393</v>
+      </c>
+      <c r="C64" t="s">
+        <v>449</v>
+      </c>
+      <c r="D64" t="s">
+        <v>458</v>
+      </c>
+      <c r="E64" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>385</v>
+      </c>
+      <c r="B65" t="s">
+        <v>394</v>
+      </c>
+      <c r="C65" t="s">
+        <v>449</v>
+      </c>
+      <c r="D65" t="s">
+        <v>458</v>
+      </c>
+      <c r="E65" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>385</v>
+      </c>
+      <c r="B66" t="s">
+        <v>395</v>
+      </c>
+      <c r="C66" t="s">
+        <v>449</v>
+      </c>
+      <c r="D66" t="s">
+        <v>458</v>
+      </c>
+      <c r="E66" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>386</v>
+      </c>
+      <c r="B67" t="s">
+        <v>391</v>
+      </c>
+      <c r="C67" t="s">
+        <v>449</v>
+      </c>
+      <c r="D67" t="s">
+        <v>457</v>
+      </c>
+      <c r="E67" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>386</v>
+      </c>
+      <c r="B68" t="s">
+        <v>392</v>
+      </c>
+      <c r="C68">
+        <v>0.54545454545454497</v>
+      </c>
+      <c r="D68" t="s">
+        <v>457</v>
+      </c>
+      <c r="E68" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>386</v>
+      </c>
+      <c r="B69" t="s">
+        <v>393</v>
+      </c>
+      <c r="C69">
+        <v>0.439393939393939</v>
+      </c>
+      <c r="D69" t="s">
+        <v>457</v>
+      </c>
+      <c r="E69" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>386</v>
+      </c>
+      <c r="B70" t="s">
+        <v>394</v>
+      </c>
+      <c r="C70" t="s">
+        <v>449</v>
+      </c>
+      <c r="D70" t="s">
+        <v>457</v>
+      </c>
+      <c r="E70" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>386</v>
+      </c>
+      <c r="B71" t="s">
+        <v>395</v>
+      </c>
+      <c r="C71" t="s">
+        <v>449</v>
+      </c>
+      <c r="D71" t="s">
+        <v>457</v>
+      </c>
+      <c r="E71" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>390</v>
+      </c>
+      <c r="B72" t="s">
+        <v>391</v>
+      </c>
+      <c r="C72" t="s">
+        <v>449</v>
+      </c>
+      <c r="D72" t="s">
+        <v>457</v>
+      </c>
+      <c r="E72" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B73" t="s">
+        <v>392</v>
+      </c>
+      <c r="C73">
+        <v>0.63157894736842102</v>
+      </c>
+      <c r="D73" t="s">
+        <v>457</v>
+      </c>
+      <c r="E73" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>390</v>
+      </c>
+      <c r="B74" t="s">
+        <v>393</v>
+      </c>
+      <c r="C74">
+        <v>0.34210526315789502</v>
+      </c>
+      <c r="D74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E74" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>390</v>
+      </c>
+      <c r="B75" t="s">
+        <v>394</v>
+      </c>
+      <c r="C75" t="s">
+        <v>449</v>
+      </c>
+      <c r="D75" t="s">
+        <v>457</v>
+      </c>
+      <c r="E75" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>390</v>
+      </c>
+      <c r="B76" t="s">
+        <v>395</v>
+      </c>
+      <c r="C76" t="s">
+        <v>449</v>
+      </c>
+      <c r="D76" t="s">
+        <v>457</v>
+      </c>
+      <c r="E76" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>377</v>
+      </c>
+      <c r="B77" t="s">
+        <v>391</v>
+      </c>
+      <c r="C77" t="s">
+        <v>449</v>
+      </c>
+      <c r="D77" t="s">
+        <v>458</v>
+      </c>
+      <c r="E77" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>377</v>
+      </c>
+      <c r="B78" t="s">
+        <v>392</v>
+      </c>
+      <c r="C78">
+        <v>0.6</v>
+      </c>
+      <c r="D78" t="s">
+        <v>458</v>
+      </c>
+      <c r="E78" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>377</v>
+      </c>
+      <c r="B79" t="s">
+        <v>393</v>
+      </c>
+      <c r="C79">
+        <v>0.3</v>
+      </c>
+      <c r="D79" t="s">
+        <v>458</v>
+      </c>
+      <c r="E79" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>377</v>
+      </c>
+      <c r="B80" t="s">
+        <v>394</v>
+      </c>
+      <c r="C80" t="s">
+        <v>449</v>
+      </c>
+      <c r="D80" t="s">
+        <v>458</v>
+      </c>
+      <c r="E80" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>377</v>
+      </c>
+      <c r="B81" t="s">
+        <v>395</v>
+      </c>
+      <c r="C81" t="s">
+        <v>449</v>
+      </c>
+      <c r="D81" t="s">
+        <v>458</v>
+      </c>
+      <c r="E81" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>378</v>
+      </c>
+      <c r="B82" t="s">
+        <v>391</v>
+      </c>
+      <c r="C82" t="s">
+        <v>449</v>
+      </c>
+      <c r="D82" t="s">
+        <v>457</v>
+      </c>
+      <c r="E82" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>378</v>
+      </c>
+      <c r="B83" t="s">
+        <v>392</v>
+      </c>
+      <c r="C83" s="1">
+        <v>0.81578947368421095</v>
+      </c>
+      <c r="D83" t="s">
+        <v>457</v>
+      </c>
+      <c r="E83" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>378</v>
+      </c>
+      <c r="B84" t="s">
+        <v>393</v>
+      </c>
+      <c r="C84" t="s">
+        <v>449</v>
+      </c>
+      <c r="D84" t="s">
+        <v>457</v>
+      </c>
+      <c r="E84" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>378</v>
+      </c>
+      <c r="B85" t="s">
+        <v>394</v>
+      </c>
+      <c r="C85" t="s">
+        <v>449</v>
+      </c>
+      <c r="D85" t="s">
+        <v>457</v>
+      </c>
+      <c r="E85" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>378</v>
+      </c>
+      <c r="B86" t="s">
+        <v>395</v>
+      </c>
+      <c r="C86" t="s">
+        <v>449</v>
+      </c>
+      <c r="D86" t="s">
+        <v>457</v>
+      </c>
+      <c r="E86" t="s">
+        <v>468</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:C102">
+    <sortCondition ref="A2:A102"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>